<commit_message>
Generalize for non-CJEU uses
Also shift standard from RMySQL to RMariaDB, allowing for UTF-8.
</commit_message>
<xml_diff>
--- a/systemdata/variable_list.xlsx
+++ b/systemdata/variable_list.xlsx
@@ -276,10 +276,10 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.66"/>
@@ -754,6 +754,9 @@
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>